<commit_message>
Calibration and validation with Gratnig
</commit_message>
<xml_diff>
--- a/Grating_params.xlsx
+++ b/Grating_params.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Scripts\VisExp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="145621"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -47,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -353,7 +345,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -364,7 +356,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates to many funtion trying to use xrite for screen calibration
</commit_message>
<xml_diff>
--- a/Grating_params.xlsx
+++ b/Grating_params.xlsx
@@ -33,7 +33,7 @@
     <t>freq</t>
   </si>
   <si>
-    <t>[-0.66, 0.66]</t>
+    <t>[0, 0]</t>
   </si>
 </sst>
 </file>
@@ -345,7 +345,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -356,7 +356,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -383,7 +383,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -397,7 +397,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -411,7 +411,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -425,7 +425,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -439,7 +439,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -453,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -467,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -481,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0.03</v>
       </c>
       <c r="D9">
         <v>1</v>

</xml_diff>